<commit_message>
many machines to many machines
</commit_message>
<xml_diff>
--- a/LineData.xlsx
+++ b/LineData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
   <si>
     <t>Config</t>
   </si>
@@ -107,7 +107,7 @@
     <t>M1</t>
   </si>
   <si>
-    <t>M3</t>
+    <t>["M2", "M3"]</t>
   </si>
   <si>
     <t>3600*24</t>
@@ -116,7 +116,22 @@
     <t>M2</t>
   </si>
   <si>
+    <t>["M4", "M5"]</t>
+  </si>
+  <si>
+    <t>M3</t>
+  </si>
+  <si>
     <t>M4</t>
+  </si>
+  <si>
+    <t>M6</t>
+  </si>
+  <si>
+    <t>M5</t>
+  </si>
+  <si>
+    <t>M7</t>
   </si>
   <si>
     <t>END</t>
@@ -615,7 +630,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:AJ501"/>
+  <dimension ref="A1:AJ499"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -797,7 +812,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F3" s="14">
         <v>1</v>
@@ -847,7 +862,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="13" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B4" s="14">
         <v>100</v>
@@ -909,7 +924,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
       <c r="A5" s="13" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B5" s="14">
         <v>100</v>
@@ -921,7 +936,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F5" s="14">
         <v>1</v>
@@ -970,18 +985,42 @@
       <c r="AJ5" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="12"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
+      <c r="A6" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="14">
+        <v>100</v>
+      </c>
+      <c r="C6" s="14">
+        <v>1</v>
+      </c>
+      <c r="D6" s="14">
+        <v>1</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="14">
+        <v>1</v>
+      </c>
+      <c r="G6" s="14">
+        <v>0</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" s="14">
+        <v>3600</v>
+      </c>
+      <c r="J6" s="14">
+        <v>100</v>
+      </c>
+      <c r="K6" s="15">
+        <v>10</v>
+      </c>
+      <c r="L6" s="6">
+        <v>5</v>
+      </c>
       <c r="M6" s="12"/>
       <c r="N6" s="12"/>
       <c r="O6" s="12"/>
@@ -1007,19 +1046,43 @@
       <c r="AI6" s="12"/>
       <c r="AJ6" s="12"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="12"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="15"/>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="24.75">
+      <c r="A7" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="14">
+        <v>100</v>
+      </c>
+      <c r="C7" s="14">
+        <v>1</v>
+      </c>
+      <c r="D7" s="14">
+        <v>1</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="14">
+        <v>1</v>
+      </c>
+      <c r="G7" s="14">
+        <v>0</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" s="14">
+        <v>3600</v>
+      </c>
+      <c r="J7" s="14">
+        <v>100</v>
+      </c>
+      <c r="K7" s="15">
+        <v>10</v>
+      </c>
+      <c r="L7" s="6">
+        <v>6</v>
+      </c>
       <c r="M7" s="12"/>
       <c r="N7" s="12"/>
       <c r="O7" s="12"/>
@@ -1046,18 +1109,42 @@
       <c r="AJ7" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="12"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
+      <c r="A8" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="14">
+        <v>100</v>
+      </c>
+      <c r="C8" s="14">
+        <v>1</v>
+      </c>
+      <c r="D8" s="14">
+        <v>1</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="14">
+        <v>1</v>
+      </c>
+      <c r="G8" s="14">
+        <v>0</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" s="14">
+        <v>3600</v>
+      </c>
+      <c r="J8" s="14">
+        <v>100</v>
+      </c>
+      <c r="K8" s="15">
+        <v>10</v>
+      </c>
+      <c r="L8" s="6">
+        <v>7</v>
+      </c>
       <c r="M8" s="12"/>
       <c r="N8" s="12"/>
       <c r="O8" s="12"/>
@@ -19741,82 +19828,6 @@
       <c r="AI499" s="12"/>
       <c r="AJ499" s="12"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="500" customHeight="1" ht="18.75">
-      <c r="A500" s="12"/>
-      <c r="B500" s="15"/>
-      <c r="C500" s="15"/>
-      <c r="D500" s="15"/>
-      <c r="E500" s="12"/>
-      <c r="F500" s="15"/>
-      <c r="G500" s="15"/>
-      <c r="H500" s="12"/>
-      <c r="I500" s="15"/>
-      <c r="J500" s="15"/>
-      <c r="K500" s="15"/>
-      <c r="L500" s="15"/>
-      <c r="M500" s="12"/>
-      <c r="N500" s="12"/>
-      <c r="O500" s="12"/>
-      <c r="P500" s="12"/>
-      <c r="Q500" s="12"/>
-      <c r="R500" s="12"/>
-      <c r="S500" s="12"/>
-      <c r="T500" s="12"/>
-      <c r="U500" s="12"/>
-      <c r="V500" s="12"/>
-      <c r="W500" s="12"/>
-      <c r="X500" s="12"/>
-      <c r="Y500" s="12"/>
-      <c r="Z500" s="12"/>
-      <c r="AA500" s="12"/>
-      <c r="AB500" s="12"/>
-      <c r="AC500" s="12"/>
-      <c r="AD500" s="12"/>
-      <c r="AE500" s="12"/>
-      <c r="AF500" s="12"/>
-      <c r="AG500" s="12"/>
-      <c r="AH500" s="12"/>
-      <c r="AI500" s="12"/>
-      <c r="AJ500" s="12"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="501" customHeight="1" ht="18.75">
-      <c r="A501" s="12"/>
-      <c r="B501" s="15"/>
-      <c r="C501" s="15"/>
-      <c r="D501" s="15"/>
-      <c r="E501" s="12"/>
-      <c r="F501" s="15"/>
-      <c r="G501" s="15"/>
-      <c r="H501" s="12"/>
-      <c r="I501" s="15"/>
-      <c r="J501" s="15"/>
-      <c r="K501" s="15"/>
-      <c r="L501" s="15"/>
-      <c r="M501" s="12"/>
-      <c r="N501" s="12"/>
-      <c r="O501" s="12"/>
-      <c r="P501" s="12"/>
-      <c r="Q501" s="12"/>
-      <c r="R501" s="12"/>
-      <c r="S501" s="12"/>
-      <c r="T501" s="12"/>
-      <c r="U501" s="12"/>
-      <c r="V501" s="12"/>
-      <c r="W501" s="12"/>
-      <c r="X501" s="12"/>
-      <c r="Y501" s="12"/>
-      <c r="Z501" s="12"/>
-      <c r="AA501" s="12"/>
-      <c r="AB501" s="12"/>
-      <c r="AC501" s="12"/>
-      <c r="AD501" s="12"/>
-      <c r="AE501" s="12"/>
-      <c r="AF501" s="12"/>
-      <c r="AG501" s="12"/>
-      <c r="AH501" s="12"/>
-      <c r="AI501" s="12"/>
-      <c r="AJ501" s="12"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
add forcast data generation
</commit_message>
<xml_diff>
--- a/LineData.xlsx
+++ b/LineData.xlsx
@@ -747,10 +747,10 @@
         <v>30</v>
       </c>
       <c r="F2" s="14">
-        <v>900</v>
+        <v>1</v>
       </c>
       <c r="G2" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2" s="13" t="s">
         <v>31</v>
@@ -758,9 +758,11 @@
       <c r="I2" s="14">
         <v>3600</v>
       </c>
-      <c r="J2" s="14"/>
+      <c r="J2" s="14">
+        <v>100</v>
+      </c>
       <c r="K2" s="15">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="L2" s="14">
         <v>1</v>
@@ -807,10 +809,10 @@
         <v>32</v>
       </c>
       <c r="F3" s="14">
-        <v>173</v>
+        <v>1</v>
       </c>
       <c r="G3" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3" s="13" t="s">
         <v>31</v>
@@ -822,7 +824,7 @@
         <v>100</v>
       </c>
       <c r="K3" s="15">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="L3" s="14">
         <v>2</v>
@@ -872,7 +874,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4" s="13" t="s">
         <v>31</v>
@@ -884,7 +886,7 @@
         <v>100</v>
       </c>
       <c r="K4" s="15">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="L4" s="6">
         <v>3</v>
@@ -934,7 +936,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5" s="13" t="s">
         <v>31</v>
@@ -946,7 +948,7 @@
         <v>100</v>
       </c>
       <c r="K5" s="15">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="L5" s="6">
         <v>4</v>
@@ -996,7 +998,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6" s="13" t="s">
         <v>31</v>
@@ -1008,7 +1010,7 @@
         <v>100</v>
       </c>
       <c r="K6" s="15">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="L6" s="6">
         <v>5</v>
@@ -1058,7 +1060,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7" s="13" t="s">
         <v>31</v>
@@ -1070,7 +1072,7 @@
         <v>100</v>
       </c>
       <c r="K7" s="15">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="L7" s="6">
         <v>6</v>
@@ -1132,7 +1134,7 @@
         <v>100</v>
       </c>
       <c r="K8" s="15">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="L8" s="15">
         <v>7</v>
@@ -19845,7 +19847,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="6">
-        <v>200000</v>
+        <v>1000</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">

</xml_diff>

<commit_message>
all set for demos
</commit_message>
<xml_diff>
--- a/LineData.xlsx
+++ b/LineData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="52">
   <si>
     <t>Available Strategies</t>
   </si>
@@ -156,7 +156,7 @@
     <t>M8</t>
   </si>
   <si>
-    <t>M12</t>
+    <t>["M11", "M12"]</t>
   </si>
   <si>
     <t>M9</t>
@@ -169,6 +169,9 @@
   </si>
   <si>
     <t>END</t>
+  </si>
+  <si>
+    <t>M12</t>
   </si>
 </sst>
 </file>
@@ -740,7 +743,7 @@
     <col min="36" max="36" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="13" t="s">
         <v>23</v>
       </c>
@@ -1436,7 +1439,7 @@
         <v>1</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="F12" s="17">
         <v>1</v>
@@ -1486,7 +1489,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="20.25">
       <c r="A13" s="16" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B13" s="17">
         <v>50</v>

</xml_diff>

<commit_message>
included reporting with no loading
</commit_message>
<xml_diff>
--- a/LineData.xlsx
+++ b/LineData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Line Data"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
   <si>
     <t>Available Strategies</t>
   </si>
@@ -129,19 +129,16 @@
     <t>M1</t>
   </si>
   <si>
-    <t>["M3", "M4","M5","M6", "M7", "M8"]</t>
+    <t>["M3", "M4","M5"]</t>
   </si>
   <si>
     <t>3600*24*2</t>
   </si>
   <si>
-    <t>M2</t>
-  </si>
-  <si>
     <t>M3</t>
   </si>
   <si>
-    <t>M9</t>
+    <t>M6</t>
   </si>
   <si>
     <t>M4</t>
@@ -150,37 +147,13 @@
     <t>M5</t>
   </si>
   <si>
-    <t>M6</t>
-  </si>
-  <si>
     <t>M7</t>
   </si>
   <si>
     <t>M8</t>
   </si>
   <si>
-    <t>["M10", "M11","M12","M13","M14","M15"]</t>
-  </si>
-  <si>
-    <t>M10</t>
-  </si>
-  <si>
     <t>END</t>
-  </si>
-  <si>
-    <t>M11</t>
-  </si>
-  <si>
-    <t>M12</t>
-  </si>
-  <si>
-    <t>M13</t>
-  </si>
-  <si>
-    <t>M14</t>
-  </si>
-  <si>
-    <t>M15</t>
   </si>
 </sst>
 </file>
@@ -400,8 +373,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:L4" displayName="Table2" name="Table2" id="1" totalsRowShown="0">
-  <autoFilter ref="A1:L4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:L3" displayName="Table2" name="Table2" id="1" totalsRowShown="0">
+  <autoFilter ref="A1:L3"/>
   <tableColumns count="12">
     <tableColumn name="Machine" id="1"/>
     <tableColumn name="CT" id="2"/>
@@ -708,9 +681,9 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:AJ485"/>
+  <dimension ref="A1:AJ484"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -819,7 +792,7 @@
         <v>36</v>
       </c>
       <c r="B2" s="17">
-        <v>2052</v>
+        <v>50</v>
       </c>
       <c r="C2" s="17">
         <v>1</v>
@@ -881,7 +854,7 @@
         <v>39</v>
       </c>
       <c r="B3" s="17">
-        <v>2052</v>
+        <v>1260</v>
       </c>
       <c r="C3" s="17">
         <v>1</v>
@@ -890,7 +863,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F3" s="17">
         <v>1</v>
@@ -905,7 +878,7 @@
         <v>3600</v>
       </c>
       <c r="J3" s="17">
-        <v>100</v>
+        <v>180</v>
       </c>
       <c r="K3" s="17">
         <v>0</v>
@@ -940,7 +913,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B4" s="17">
         <v>1260</v>
@@ -952,7 +925,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F4" s="17">
         <v>1</v>
@@ -972,7 +945,7 @@
       <c r="K4" s="17">
         <v>0</v>
       </c>
-      <c r="L4" s="17">
+      <c r="L4" s="8">
         <v>3</v>
       </c>
       <c r="M4" s="1"/>
@@ -1014,7 +987,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F5" s="17">
         <v>1</v>
@@ -1029,7 +1002,7 @@
         <v>3600</v>
       </c>
       <c r="J5" s="17">
-        <v>180</v>
+        <v>260</v>
       </c>
       <c r="K5" s="17">
         <v>0</v>
@@ -1064,10 +1037,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="16" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B6" s="17">
-        <v>1260</v>
+        <v>25</v>
       </c>
       <c r="C6" s="17">
         <v>1</v>
@@ -1076,7 +1049,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F6" s="17">
         <v>1</v>
@@ -1126,10 +1099,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B7" s="17">
-        <v>1260</v>
+        <v>100</v>
       </c>
       <c r="C7" s="17">
         <v>1</v>
@@ -1138,7 +1111,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F7" s="17">
         <v>1</v>
@@ -1153,7 +1126,7 @@
         <v>3600</v>
       </c>
       <c r="J7" s="17">
-        <v>260</v>
+        <v>340</v>
       </c>
       <c r="K7" s="17">
         <v>0</v>
@@ -1188,10 +1161,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8" s="17">
-        <v>1260</v>
+        <v>10</v>
       </c>
       <c r="C8" s="17">
         <v>1</v>
@@ -1200,7 +1173,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="F8" s="17">
         <v>1</v>
@@ -1249,42 +1222,18 @@
       <c r="AJ8" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="B9" s="17">
-        <v>1260</v>
-      </c>
-      <c r="C9" s="17">
-        <v>1</v>
-      </c>
-      <c r="D9" s="17">
-        <v>1</v>
-      </c>
-      <c r="E9" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="F9" s="17">
-        <v>1</v>
-      </c>
-      <c r="G9" s="17">
-        <v>0</v>
-      </c>
-      <c r="H9" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="I9" s="17">
-        <v>3600</v>
-      </c>
-      <c r="J9" s="17">
-        <v>340</v>
-      </c>
-      <c r="K9" s="17">
-        <v>0</v>
-      </c>
-      <c r="L9" s="8">
-        <v>8</v>
-      </c>
+      <c r="A9" s="16"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="8"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
@@ -1311,42 +1260,18 @@
       <c r="AJ9" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" s="17">
-        <v>54</v>
-      </c>
-      <c r="C10" s="17">
-        <v>1</v>
-      </c>
-      <c r="D10" s="17">
-        <v>1</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="F10" s="17">
-        <v>1</v>
-      </c>
-      <c r="G10" s="17">
-        <v>0</v>
-      </c>
-      <c r="H10" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="I10" s="17">
-        <v>3600</v>
-      </c>
-      <c r="J10" s="17">
-        <v>-210</v>
-      </c>
-      <c r="K10" s="17">
-        <v>0</v>
-      </c>
-      <c r="L10" s="8">
-        <v>9</v>
-      </c>
+      <c r="A10" s="16"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="8"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
@@ -1373,42 +1298,18 @@
       <c r="AJ10" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
-      <c r="A11" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" s="17">
-        <v>3420</v>
-      </c>
-      <c r="C11" s="17">
-        <v>1</v>
-      </c>
-      <c r="D11" s="17">
-        <v>1</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="F11" s="17">
-        <v>1</v>
-      </c>
-      <c r="G11" s="17">
-        <v>0</v>
-      </c>
-      <c r="H11" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="I11" s="17">
-        <v>3600</v>
-      </c>
-      <c r="J11" s="17">
-        <v>180</v>
-      </c>
-      <c r="K11" s="17">
-        <v>0</v>
-      </c>
-      <c r="L11" s="8">
-        <v>10</v>
-      </c>
+      <c r="A11" s="16"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="8"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
@@ -1435,42 +1336,18 @@
       <c r="AJ11" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
-      <c r="A12" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B12" s="17">
-        <v>3420</v>
-      </c>
-      <c r="C12" s="17">
-        <v>1</v>
-      </c>
-      <c r="D12" s="17">
-        <v>1</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="F12" s="17">
-        <v>1</v>
-      </c>
-      <c r="G12" s="17">
-        <v>0</v>
-      </c>
-      <c r="H12" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="I12" s="17">
-        <v>3600</v>
-      </c>
-      <c r="J12" s="17">
-        <v>180</v>
-      </c>
-      <c r="K12" s="17">
-        <v>0</v>
-      </c>
-      <c r="L12" s="8">
-        <v>11</v>
-      </c>
+      <c r="A12" s="16"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="8"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
@@ -1497,42 +1374,18 @@
       <c r="AJ12" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
-      <c r="A13" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="B13" s="17">
-        <v>3420</v>
-      </c>
-      <c r="C13" s="17">
-        <v>1</v>
-      </c>
-      <c r="D13" s="17">
-        <v>1</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="F13" s="17">
-        <v>1</v>
-      </c>
-      <c r="G13" s="17">
-        <v>0</v>
-      </c>
-      <c r="H13" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="I13" s="17">
-        <v>3600</v>
-      </c>
-      <c r="J13" s="17">
-        <v>260</v>
-      </c>
-      <c r="K13" s="17">
-        <v>0</v>
-      </c>
-      <c r="L13" s="8">
-        <v>12</v>
-      </c>
+      <c r="A13" s="16"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="8"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
@@ -1559,42 +1412,18 @@
       <c r="AJ13" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
-      <c r="A14" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="B14" s="17">
-        <v>3420</v>
-      </c>
-      <c r="C14" s="17">
-        <v>1</v>
-      </c>
-      <c r="D14" s="17">
-        <v>1</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="F14" s="17">
-        <v>1</v>
-      </c>
-      <c r="G14" s="17">
-        <v>0</v>
-      </c>
-      <c r="H14" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="I14" s="17">
-        <v>3600</v>
-      </c>
-      <c r="J14" s="17">
-        <v>260</v>
-      </c>
-      <c r="K14" s="17">
-        <v>0</v>
-      </c>
-      <c r="L14" s="8">
-        <v>13</v>
-      </c>
+      <c r="A14" s="16"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="8"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
@@ -1621,42 +1450,18 @@
       <c r="AJ14" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
-      <c r="A15" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="B15" s="17">
-        <v>3420</v>
-      </c>
-      <c r="C15" s="17">
-        <v>1</v>
-      </c>
-      <c r="D15" s="17">
-        <v>1</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="F15" s="17">
-        <v>1</v>
-      </c>
-      <c r="G15" s="17">
-        <v>0</v>
-      </c>
-      <c r="H15" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="I15" s="17">
-        <v>3600</v>
-      </c>
-      <c r="J15" s="17">
-        <v>340</v>
-      </c>
-      <c r="K15" s="17">
-        <v>0</v>
-      </c>
-      <c r="L15" s="8">
-        <v>14</v>
-      </c>
+      <c r="A15" s="16"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="8"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
@@ -1682,43 +1487,19 @@
       <c r="AI15" s="1"/>
       <c r="AJ15" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
-      <c r="A16" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="B16" s="17">
-        <v>3420</v>
-      </c>
-      <c r="C16" s="17">
-        <v>1</v>
-      </c>
-      <c r="D16" s="17">
-        <v>1</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="F16" s="17">
-        <v>1</v>
-      </c>
-      <c r="G16" s="17">
-        <v>0</v>
-      </c>
-      <c r="H16" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="I16" s="17">
-        <v>3600</v>
-      </c>
-      <c r="J16" s="17">
-        <v>340</v>
-      </c>
-      <c r="K16" s="17">
-        <v>0</v>
-      </c>
-      <c r="L16" s="8">
-        <v>15</v>
-      </c>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="20.25">
+      <c r="A16" s="16"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="8"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
@@ -1744,19 +1525,19 @@
       <c r="AI16" s="1"/>
       <c r="AJ16" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="20.25">
-      <c r="A17" s="16"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="8"/>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+      <c r="A17" s="1"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
@@ -2580,7 +2361,7 @@
       <c r="AI38" s="1"/>
       <c r="AJ38" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
       <c r="A39" s="1"/>
       <c r="B39" s="18"/>
       <c r="C39" s="18"/>
@@ -19528,44 +19309,6 @@
       <c r="AI484" s="1"/>
       <c r="AJ484" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="485" customHeight="1" ht="18.75">
-      <c r="A485" s="1"/>
-      <c r="B485" s="18"/>
-      <c r="C485" s="18"/>
-      <c r="D485" s="18"/>
-      <c r="E485" s="1"/>
-      <c r="F485" s="18"/>
-      <c r="G485" s="18"/>
-      <c r="H485" s="1"/>
-      <c r="I485" s="18"/>
-      <c r="J485" s="18"/>
-      <c r="K485" s="18"/>
-      <c r="L485" s="18"/>
-      <c r="M485" s="1"/>
-      <c r="N485" s="1"/>
-      <c r="O485" s="1"/>
-      <c r="P485" s="1"/>
-      <c r="Q485" s="1"/>
-      <c r="R485" s="1"/>
-      <c r="S485" s="1"/>
-      <c r="T485" s="1"/>
-      <c r="U485" s="1"/>
-      <c r="V485" s="1"/>
-      <c r="W485" s="1"/>
-      <c r="X485" s="1"/>
-      <c r="Y485" s="1"/>
-      <c r="Z485" s="1"/>
-      <c r="AA485" s="1"/>
-      <c r="AB485" s="1"/>
-      <c r="AC485" s="1"/>
-      <c r="AD485" s="1"/>
-      <c r="AE485" s="1"/>
-      <c r="AF485" s="1"/>
-      <c r="AG485" s="1"/>
-      <c r="AH485" s="1"/>
-      <c r="AI485" s="1"/>
-      <c r="AJ485" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -19581,7 +19324,7 @@
   </sheetPr>
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
reset shift to be solved
</commit_message>
<xml_diff>
--- a/LineData.xlsx
+++ b/LineData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="74">
   <si>
     <t>Available Strategies</t>
   </si>
@@ -196,6 +196,9 @@
   </si>
   <si>
     <t>["M10", "M11","M12","M13","M14","M15"]</t>
+  </si>
+  <si>
+    <t>3600*24*6</t>
   </si>
   <si>
     <t>M10</t>
@@ -901,7 +904,7 @@
         <v>42</v>
       </c>
       <c r="J2" s="17">
-        <v>3600</v>
+        <v>1200</v>
       </c>
       <c r="K2" s="17">
         <v>100</v>
@@ -965,7 +968,7 @@
         <v>42</v>
       </c>
       <c r="J3" s="17">
-        <v>3600</v>
+        <v>1200</v>
       </c>
       <c r="K3" s="17">
         <v>100</v>
@@ -1029,7 +1032,7 @@
         <v>42</v>
       </c>
       <c r="J4" s="17">
-        <v>3600</v>
+        <v>1200</v>
       </c>
       <c r="K4" s="17">
         <v>180</v>
@@ -1093,7 +1096,7 @@
         <v>42</v>
       </c>
       <c r="J5" s="17">
-        <v>3600</v>
+        <v>1200</v>
       </c>
       <c r="K5" s="17">
         <v>180</v>
@@ -1157,7 +1160,7 @@
         <v>42</v>
       </c>
       <c r="J6" s="17">
-        <v>3600</v>
+        <v>1200</v>
       </c>
       <c r="K6" s="17">
         <v>260</v>
@@ -1221,7 +1224,7 @@
         <v>42</v>
       </c>
       <c r="J7" s="17">
-        <v>3600</v>
+        <v>1200</v>
       </c>
       <c r="K7" s="17">
         <v>260</v>
@@ -1285,7 +1288,7 @@
         <v>42</v>
       </c>
       <c r="J8" s="17">
-        <v>3600</v>
+        <v>1200</v>
       </c>
       <c r="K8" s="17">
         <v>340</v>
@@ -1349,7 +1352,7 @@
         <v>42</v>
       </c>
       <c r="J9" s="17">
-        <v>3600</v>
+        <v>1200</v>
       </c>
       <c r="K9" s="17">
         <v>340</v>
@@ -1410,10 +1413,10 @@
         <v>0</v>
       </c>
       <c r="I10" s="16" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="J10" s="17">
-        <v>3600</v>
+        <v>1200</v>
       </c>
       <c r="K10" s="17">
         <v>-210</v>
@@ -1450,10 +1453,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="16" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C11" s="17">
         <v>3420</v>
@@ -1465,7 +1468,7 @@
         <v>1</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G11" s="17">
         <v>1</v>
@@ -1477,7 +1480,7 @@
         <v>42</v>
       </c>
       <c r="J11" s="17">
-        <v>3600</v>
+        <v>1200</v>
       </c>
       <c r="K11" s="17">
         <v>180</v>
@@ -1514,10 +1517,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="16" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C12" s="17">
         <v>3420</v>
@@ -1529,7 +1532,7 @@
         <v>1</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G12" s="17">
         <v>1</v>
@@ -1541,7 +1544,7 @@
         <v>42</v>
       </c>
       <c r="J12" s="17">
-        <v>3600</v>
+        <v>1200</v>
       </c>
       <c r="K12" s="17">
         <v>180</v>
@@ -1578,10 +1581,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="16" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C13" s="17">
         <v>3420</v>
@@ -1593,7 +1596,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="16" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G13" s="17">
         <v>1</v>
@@ -1605,7 +1608,7 @@
         <v>42</v>
       </c>
       <c r="J13" s="17">
-        <v>3600</v>
+        <v>1200</v>
       </c>
       <c r="K13" s="17">
         <v>260</v>
@@ -1642,10 +1645,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="16" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C14" s="17">
         <v>3420</v>
@@ -1657,7 +1660,7 @@
         <v>1</v>
       </c>
       <c r="F14" s="16" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G14" s="17">
         <v>1</v>
@@ -1669,7 +1672,7 @@
         <v>42</v>
       </c>
       <c r="J14" s="17">
-        <v>3600</v>
+        <v>1200</v>
       </c>
       <c r="K14" s="17">
         <v>260</v>
@@ -1706,10 +1709,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="16" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C15" s="17">
         <v>3420</v>
@@ -1721,7 +1724,7 @@
         <v>1</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G15" s="17">
         <v>1</v>
@@ -1733,7 +1736,7 @@
         <v>42</v>
       </c>
       <c r="J15" s="17">
-        <v>3600</v>
+        <v>1200</v>
       </c>
       <c r="K15" s="17">
         <v>340</v>
@@ -1770,10 +1773,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="20.25">
       <c r="A16" s="16" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C16" s="17">
         <v>3420</v>
@@ -1785,7 +1788,7 @@
         <v>1</v>
       </c>
       <c r="F16" s="16" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G16" s="17">
         <v>1</v>
@@ -1797,7 +1800,7 @@
         <v>42</v>
       </c>
       <c r="J16" s="17">
-        <v>3600</v>
+        <v>1200</v>
       </c>
       <c r="K16" s="17">
         <v>340</v>

</xml_diff>

<commit_message>
multi-ref started to work
</commit_message>
<xml_diff>
--- a/LineData.xlsx
+++ b/LineData.xlsx
@@ -809,7 +809,7 @@
     <col min="36" max="36" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
       <c r="A1" s="9" t="s">
         <v>25</v>
       </c>
@@ -875,7 +875,7 @@
       <c r="AI1" s="1"/>
       <c r="AJ1" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="16" t="s">
         <v>39</v>
       </c>
@@ -904,7 +904,7 @@
         <v>42</v>
       </c>
       <c r="J2" s="17">
-        <v>1200</v>
+        <v>3600</v>
       </c>
       <c r="K2" s="17">
         <v>100</v>
@@ -939,7 +939,7 @@
       <c r="AI2" s="1"/>
       <c r="AJ2" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="16" t="s">
         <v>43</v>
       </c>
@@ -968,7 +968,7 @@
         <v>42</v>
       </c>
       <c r="J3" s="17">
-        <v>1200</v>
+        <v>3600</v>
       </c>
       <c r="K3" s="17">
         <v>100</v>
@@ -1003,7 +1003,7 @@
       <c r="AI3" s="1"/>
       <c r="AJ3" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="16" t="s">
         <v>45</v>
       </c>
@@ -1032,7 +1032,7 @@
         <v>42</v>
       </c>
       <c r="J4" s="17">
-        <v>1200</v>
+        <v>3600</v>
       </c>
       <c r="K4" s="17">
         <v>180</v>
@@ -1067,7 +1067,7 @@
       <c r="AI4" s="1"/>
       <c r="AJ4" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="16" t="s">
         <v>48</v>
       </c>
@@ -1096,7 +1096,7 @@
         <v>42</v>
       </c>
       <c r="J5" s="17">
-        <v>1200</v>
+        <v>3600</v>
       </c>
       <c r="K5" s="17">
         <v>180</v>
@@ -1131,7 +1131,7 @@
       <c r="AI5" s="1"/>
       <c r="AJ5" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="16" t="s">
         <v>50</v>
       </c>
@@ -1160,7 +1160,7 @@
         <v>42</v>
       </c>
       <c r="J6" s="17">
-        <v>1200</v>
+        <v>3600</v>
       </c>
       <c r="K6" s="17">
         <v>260</v>
@@ -1195,7 +1195,7 @@
       <c r="AI6" s="1"/>
       <c r="AJ6" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="16" t="s">
         <v>52</v>
       </c>
@@ -1224,7 +1224,7 @@
         <v>42</v>
       </c>
       <c r="J7" s="17">
-        <v>1200</v>
+        <v>3600</v>
       </c>
       <c r="K7" s="17">
         <v>260</v>
@@ -1259,7 +1259,7 @@
       <c r="AI7" s="1"/>
       <c r="AJ7" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="16" t="s">
         <v>54</v>
       </c>
@@ -1288,7 +1288,7 @@
         <v>42</v>
       </c>
       <c r="J8" s="17">
-        <v>1200</v>
+        <v>3600</v>
       </c>
       <c r="K8" s="17">
         <v>340</v>
@@ -1323,7 +1323,7 @@
       <c r="AI8" s="1"/>
       <c r="AJ8" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="16" t="s">
         <v>56</v>
       </c>
@@ -1352,7 +1352,7 @@
         <v>42</v>
       </c>
       <c r="J9" s="17">
-        <v>1200</v>
+        <v>3600</v>
       </c>
       <c r="K9" s="17">
         <v>340</v>
@@ -1387,7 +1387,7 @@
       <c r="AI9" s="1"/>
       <c r="AJ9" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="16" t="s">
         <v>47</v>
       </c>
@@ -1416,7 +1416,7 @@
         <v>60</v>
       </c>
       <c r="J10" s="17">
-        <v>1200</v>
+        <v>3600</v>
       </c>
       <c r="K10" s="17">
         <v>-210</v>
@@ -1451,7 +1451,7 @@
       <c r="AI10" s="1"/>
       <c r="AJ10" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="16" t="s">
         <v>61</v>
       </c>
@@ -1480,7 +1480,7 @@
         <v>42</v>
       </c>
       <c r="J11" s="17">
-        <v>1200</v>
+        <v>3600</v>
       </c>
       <c r="K11" s="17">
         <v>180</v>
@@ -1515,7 +1515,7 @@
       <c r="AI11" s="1"/>
       <c r="AJ11" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="16" t="s">
         <v>64</v>
       </c>
@@ -1544,7 +1544,7 @@
         <v>42</v>
       </c>
       <c r="J12" s="17">
-        <v>1200</v>
+        <v>3600</v>
       </c>
       <c r="K12" s="17">
         <v>180</v>
@@ -1579,7 +1579,7 @@
       <c r="AI12" s="1"/>
       <c r="AJ12" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="16" t="s">
         <v>66</v>
       </c>
@@ -1608,7 +1608,7 @@
         <v>42</v>
       </c>
       <c r="J13" s="17">
-        <v>1200</v>
+        <v>3600</v>
       </c>
       <c r="K13" s="17">
         <v>260</v>
@@ -1643,7 +1643,7 @@
       <c r="AI13" s="1"/>
       <c r="AJ13" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="16" t="s">
         <v>68</v>
       </c>
@@ -1672,7 +1672,7 @@
         <v>42</v>
       </c>
       <c r="J14" s="17">
-        <v>1200</v>
+        <v>3600</v>
       </c>
       <c r="K14" s="17">
         <v>260</v>
@@ -1707,7 +1707,7 @@
       <c r="AI14" s="1"/>
       <c r="AJ14" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="16" t="s">
         <v>70</v>
       </c>
@@ -1736,7 +1736,7 @@
         <v>42</v>
       </c>
       <c r="J15" s="17">
-        <v>1200</v>
+        <v>3600</v>
       </c>
       <c r="K15" s="17">
         <v>340</v>
@@ -1771,7 +1771,7 @@
       <c r="AI15" s="1"/>
       <c r="AJ15" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="16" t="s">
         <v>72</v>
       </c>
@@ -1800,7 +1800,7 @@
         <v>42</v>
       </c>
       <c r="J16" s="17">
-        <v>1200</v>
+        <v>3600</v>
       </c>
       <c r="K16" s="17">
         <v>340</v>
@@ -1835,7 +1835,7 @@
       <c r="AI16" s="1"/>
       <c r="AJ16" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="18"/>
@@ -1873,7 +1873,7 @@
       <c r="AI17" s="1"/>
       <c r="AJ17" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="18"/>
@@ -1911,7 +1911,7 @@
       <c r="AI18" s="1"/>
       <c r="AJ18" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="18"/>
@@ -1949,7 +1949,7 @@
       <c r="AI19" s="1"/>
       <c r="AJ19" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="18"/>
@@ -1987,7 +1987,7 @@
       <c r="AI20" s="1"/>
       <c r="AJ20" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="18"/>
@@ -2025,7 +2025,7 @@
       <c r="AI21" s="1"/>
       <c r="AJ21" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="18"/>
@@ -2063,7 +2063,7 @@
       <c r="AI22" s="1"/>
       <c r="AJ22" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="18"/>
@@ -2101,7 +2101,7 @@
       <c r="AI23" s="1"/>
       <c r="AJ23" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="18"/>
@@ -2139,7 +2139,7 @@
       <c r="AI24" s="1"/>
       <c r="AJ24" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="18"/>
@@ -2177,7 +2177,7 @@
       <c r="AI25" s="1"/>
       <c r="AJ25" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="18"/>
@@ -2215,7 +2215,7 @@
       <c r="AI26" s="1"/>
       <c r="AJ26" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="18"/>

</xml_diff>

<commit_message>
need for multi-ref results
</commit_message>
<xml_diff>
--- a/LineData.xlsx
+++ b/LineData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Line Data"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="76">
   <si>
     <t>Available Strategies</t>
   </si>
@@ -32,9 +32,6 @@
   </si>
   <si>
     <t>Ref A</t>
-  </si>
-  <si>
-    <t>Ref B</t>
   </si>
   <si>
     <t>Input</t>
@@ -199,7 +196,7 @@
     <t>["M3", "M4","M5","M6", "M7", "M8"]</t>
   </si>
   <si>
-    <t>3600*8*1</t>
+    <t>3600*24*5</t>
   </si>
   <si>
     <t>Flushing 2</t>
@@ -459,13 +456,13 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
@@ -475,6 +472,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
@@ -510,10 +510,7 @@
     <xf xfId="0" numFmtId="0" borderId="11" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
@@ -543,12 +540,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:C17" displayName="Tableau2" name="Tableau2" id="1" totalsRowShown="0">
-  <autoFilter ref="A1:C17"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:B17" displayName="Tableau2" name="Tableau2" id="1" totalsRowShown="0">
+  <autoFilter ref="A1:B17"/>
+  <tableColumns count="2">
     <tableColumn name="Machine" id="1"/>
     <tableColumn name="Ref A" id="2"/>
-    <tableColumn name="Ref B" id="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showColumnStripes="0" showRowStripes="1" showLastColumn="0" showFirstColumn="0"/>
 </table>
@@ -865,7 +861,7 @@
   </sheetPr>
   <dimension ref="A1:AJ484"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -908,47 +904,47 @@
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="D1" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="E1" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="F1" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="G1" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="H1" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="I1" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="J1" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="K1" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="L1" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="M1" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="M1" s="23" t="s">
+      <c r="N1" s="24" t="s">
         <v>56</v>
-      </c>
-      <c r="N1" s="24" t="s">
-        <v>57</v>
       </c>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
@@ -975,10 +971,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C2" s="8">
         <v>2052</v>
@@ -990,7 +986,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G2" s="8">
         <v>1</v>
@@ -999,7 +995,7 @@
         <v>0</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J2" s="8">
         <v>3600</v>
@@ -1039,10 +1035,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C3" s="8">
         <v>2052</v>
@@ -1054,7 +1050,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G3" s="8">
         <v>1</v>
@@ -1063,7 +1059,7 @@
         <v>0</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J3" s="8">
         <v>3600</v>
@@ -1103,10 +1099,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C4" s="8">
         <v>1260</v>
@@ -1118,7 +1114,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G4" s="8">
         <v>1</v>
@@ -1127,7 +1123,7 @@
         <v>0</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J4" s="8">
         <v>3600</v>
@@ -1167,10 +1163,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C5" s="8">
         <v>1260</v>
@@ -1182,7 +1178,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G5" s="8">
         <v>1</v>
@@ -1191,7 +1187,7 @@
         <v>0</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J5" s="8">
         <v>3600</v>
@@ -1231,10 +1227,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C6" s="8">
         <v>1260</v>
@@ -1246,7 +1242,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G6" s="8">
         <v>1</v>
@@ -1255,7 +1251,7 @@
         <v>0</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J6" s="8">
         <v>3600</v>
@@ -1295,10 +1291,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C7" s="8">
         <v>1260</v>
@@ -1310,7 +1306,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G7" s="8">
         <v>1</v>
@@ -1319,7 +1315,7 @@
         <v>0</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J7" s="8">
         <v>3600</v>
@@ -1359,10 +1355,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C8" s="8">
         <v>1260</v>
@@ -1374,7 +1370,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G8" s="8">
         <v>1</v>
@@ -1383,7 +1379,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J8" s="8">
         <v>3600</v>
@@ -1423,10 +1419,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C9" s="8">
         <v>1260</v>
@@ -1438,7 +1434,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G9" s="8">
         <v>1</v>
@@ -1447,7 +1443,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J9" s="8">
         <v>3600</v>
@@ -1487,10 +1483,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C10" s="8">
         <v>54</v>
@@ -1502,7 +1498,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G10" s="8">
         <v>1</v>
@@ -1511,7 +1507,7 @@
         <v>0</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J10" s="8">
         <v>3600</v>
@@ -1551,10 +1547,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C11" s="8">
         <v>3420</v>
@@ -1566,7 +1562,7 @@
         <v>1</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G11" s="8">
         <v>1</v>
@@ -1575,7 +1571,7 @@
         <v>0</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J11" s="8">
         <v>3600</v>
@@ -1615,10 +1611,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C12" s="8">
         <v>3420</v>
@@ -1630,7 +1626,7 @@
         <v>1</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G12" s="8">
         <v>1</v>
@@ -1639,7 +1635,7 @@
         <v>0</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J12" s="8">
         <v>3600</v>
@@ -1679,10 +1675,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C13" s="8">
         <v>3420</v>
@@ -1694,7 +1690,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G13" s="8">
         <v>1</v>
@@ -1703,7 +1699,7 @@
         <v>0</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J13" s="8">
         <v>3600</v>
@@ -1743,10 +1739,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C14" s="8">
         <v>3420</v>
@@ -1758,7 +1754,7 @@
         <v>1</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G14" s="8">
         <v>1</v>
@@ -1767,7 +1763,7 @@
         <v>0</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J14" s="8">
         <v>3600</v>
@@ -1807,10 +1803,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C15" s="8">
         <v>3420</v>
@@ -1822,7 +1818,7 @@
         <v>1</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G15" s="8">
         <v>1</v>
@@ -1831,7 +1827,7 @@
         <v>0</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J15" s="8">
         <v>3600</v>
@@ -1871,10 +1867,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="20.25">
       <c r="A16" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C16" s="8">
         <v>3420</v>
@@ -1886,7 +1882,7 @@
         <v>1</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G16" s="8">
         <v>1</v>
@@ -1895,7 +1891,7 @@
         <v>0</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J16" s="8">
         <v>3600</v>
@@ -19738,145 +19734,145 @@
   <cols>
     <col min="1" max="1" style="9" width="13.147857142857141" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="9" width="15.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="21" width="16.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="10" width="16.862142857142857" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="C1" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="12" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+      <c r="A2" s="14" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="13" t="s">
+      <c r="B2" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="C2" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="15" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+      <c r="A3" s="17"/>
+      <c r="B3" s="15" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="16"/>
-      <c r="B3" s="14" t="s">
+      <c r="C3" s="16">
+        <v>3600</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+      <c r="A4" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="15">
-        <v>3600</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="13" t="s">
+      <c r="B4" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="C4" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+      <c r="A5" s="17"/>
+      <c r="B5" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C5" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+      <c r="A6" s="17"/>
+      <c r="B6" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+      <c r="A7" s="17"/>
+      <c r="B7" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="16">
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="16"/>
-      <c r="B5" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="16"/>
-      <c r="B6" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="16"/>
-      <c r="B7" s="14" t="s">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+      <c r="A8" s="17"/>
+      <c r="B8" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C8" s="16">
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="16"/>
-      <c r="B8" s="14" t="s">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+      <c r="A9" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="15">
+      <c r="B9" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="16"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+      <c r="A10" s="17"/>
+      <c r="B10" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="16"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+      <c r="A11" s="17"/>
+      <c r="B11" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="16"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+      <c r="A12" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="16"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+      <c r="A13" s="19"/>
+      <c r="B13" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="16">
+        <v>3</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+      <c r="A14" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="16">
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="15"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="16"/>
-      <c r="B10" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="15"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
-      <c r="A11" s="16"/>
-      <c r="B11" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" s="15"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
-      <c r="A12" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="15"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
-      <c r="A13" s="18"/>
-      <c r="B13" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="15">
-        <v>3</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
-      <c r="A14" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="B14" s="14" t="s">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="20.25">
+      <c r="A15" s="21"/>
+      <c r="B15" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="20.25">
-      <c r="A15" s="20"/>
-      <c r="B15" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="16" t="s">
         <v>1</v>
       </c>
     </row>
@@ -19897,15 +19893,14 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="9" width="13.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="10.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="10" width="10.290714285714287" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -19915,183 +19910,132 @@
       <c r="B1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="8">
         <v>2052</v>
       </c>
-      <c r="C3" s="8">
-        <v>2052</v>
-      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="8">
         <v>2052</v>
       </c>
-      <c r="C4" s="8">
-        <v>2052</v>
-      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="8">
         <v>1260</v>
       </c>
-      <c r="C5" s="8">
-        <v>1260</v>
-      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="8">
         <v>1260</v>
       </c>
-      <c r="C6" s="8">
-        <v>1260</v>
-      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="8">
         <v>1260</v>
       </c>
-      <c r="C7" s="8">
-        <v>1260</v>
-      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="8">
         <v>1260</v>
       </c>
-      <c r="C8" s="8">
-        <v>1260</v>
-      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="8">
         <v>1260</v>
       </c>
-      <c r="C9" s="8">
-        <v>1260</v>
-      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" s="8">
         <v>1260</v>
       </c>
-      <c r="C10" s="8">
-        <v>1260</v>
-      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" s="8">
         <v>54</v>
       </c>
-      <c r="C11" s="8">
-        <v>54</v>
-      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" s="8">
         <v>3420</v>
       </c>
-      <c r="C12" s="8">
-        <v>3420</v>
-      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" s="8">
         <v>3420</v>
       </c>
-      <c r="C13" s="8">
-        <v>3420</v>
-      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" s="8">
         <v>3420</v>
       </c>
-      <c r="C14" s="8">
-        <v>3420</v>
-      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" s="8">
         <v>3420</v>
       </c>
-      <c r="C15" s="8">
-        <v>3420</v>
-      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16" s="8">
         <v>3420</v>
       </c>
-      <c r="C16" s="8">
-        <v>3420</v>
-      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="20.25">
       <c r="A17" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17" s="8">
-        <v>3420</v>
-      </c>
-      <c r="C17" s="8">
         <v>3420</v>
       </c>
     </row>

</xml_diff>

<commit_message>
PDP - UI + Excel file updated
</commit_message>
<xml_diff>
--- a/LineData.xlsx
+++ b/LineData.xlsx
@@ -5,26 +5,31 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danislud\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danislud\Documents\PRODynamics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9C898A01-7893-4EDB-B3F5-4E8061133302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0AFDE5D8-1D9D-43C8-A4A9-9BB4DF60813F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Line Data" sheetId="1" r:id="rId1"/>
-    <sheet name="Config" sheetId="2" r:id="rId2"/>
-    <sheet name="Multi-Ref" sheetId="3" r:id="rId3"/>
-    <sheet name="Assets" sheetId="4" r:id="rId4"/>
+    <sheet name="Multi-Ref" sheetId="3" r:id="rId2"/>
+    <sheet name="PDP-Batch-Details" sheetId="5" r:id="rId3"/>
+    <sheet name="PDP-Batch-List" sheetId="6" r:id="rId4"/>
+    <sheet name="Config" sheetId="2" r:id="rId5"/>
+    <sheet name="Assets" sheetId="4" r:id="rId6"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'PDP-Batch-Details'!$A$1:$C$1</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
   <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="81">
   <si>
     <t>Available Strategies</t>
   </si>
@@ -250,12 +255,30 @@
   <si>
     <t>Fill central storage</t>
   </si>
+  <si>
+    <t>Batch name</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Group 1</t>
+  </si>
+  <si>
+    <t>Group 2</t>
+  </si>
+  <si>
+    <t>Batchs</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -282,8 +305,16 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -299,6 +330,12 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -475,7 +512,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -546,6 +583,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -562,15 +611,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -961,7 +1001,7 @@
   </sheetPr>
   <dimension ref="A1:N481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
@@ -1011,19 +1051,19 @@
       <c r="I1" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="J1" s="33" t="s">
+      <c r="J1" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="K1" s="33" t="s">
+      <c r="K1" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="L1" s="33" t="s">
+      <c r="L1" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="M1" s="33" t="s">
+      <c r="M1" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="N1" s="33" t="s">
+      <c r="N1" s="27" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1055,17 +1095,17 @@
       <c r="I2" s="25">
         <v>1</v>
       </c>
-      <c r="J2" s="34">
+      <c r="J2" s="28">
         <v>1</v>
       </c>
-      <c r="K2" s="34">
+      <c r="K2" s="28">
         <v>0</v>
       </c>
-      <c r="L2" s="34">
+      <c r="L2" s="28">
         <v>0</v>
       </c>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34" t="b">
+      <c r="M2" s="28"/>
+      <c r="N2" s="28" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1107,7 +1147,7 @@
         <v>0</v>
       </c>
       <c r="M3" s="25"/>
-      <c r="N3" s="32" t="b">
+      <c r="N3" s="26" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1149,7 +1189,7 @@
         <v>0</v>
       </c>
       <c r="M4" s="25"/>
-      <c r="N4" s="32" t="b">
+      <c r="N4" s="26" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1191,7 +1231,7 @@
         <v>0</v>
       </c>
       <c r="M5" s="25"/>
-      <c r="N5" s="32" t="b">
+      <c r="N5" s="26" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1233,7 +1273,7 @@
         <v>0</v>
       </c>
       <c r="M6" s="25"/>
-      <c r="N6" s="32" t="b">
+      <c r="N6" s="26" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1275,7 +1315,7 @@
         <v>0</v>
       </c>
       <c r="M7" s="25"/>
-      <c r="N7" s="32" t="b">
+      <c r="N7" s="26" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1317,7 +1357,7 @@
         <v>0</v>
       </c>
       <c r="M8" s="25"/>
-      <c r="N8" s="32" t="b">
+      <c r="N8" s="26" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1359,7 +1399,7 @@
         <v>0</v>
       </c>
       <c r="M9" s="25"/>
-      <c r="N9" s="32" t="b">
+      <c r="N9" s="26" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1401,7 +1441,7 @@
         <v>0</v>
       </c>
       <c r="M10" s="25"/>
-      <c r="N10" s="32" t="b">
+      <c r="N10" s="26" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1443,7 +1483,7 @@
         <v>0</v>
       </c>
       <c r="M11" s="25"/>
-      <c r="N11" s="32" t="b">
+      <c r="N11" s="26" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1485,7 +1525,7 @@
         <v>0</v>
       </c>
       <c r="M12" s="25"/>
-      <c r="N12" s="32" t="b">
+      <c r="N12" s="26" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1527,7 +1567,7 @@
         <v>0</v>
       </c>
       <c r="M13" s="25"/>
-      <c r="N13" s="32" t="b">
+      <c r="N13" s="26" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1569,7 +1609,7 @@
         <v>0</v>
       </c>
       <c r="M14" s="25"/>
-      <c r="N14" s="32" t="b">
+      <c r="N14" s="26" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7658,179 +7698,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:C15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" style="10" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="27"/>
-      <c r="B3" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="7">
-        <v>3600</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="27"/>
-      <c r="B5" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="27"/>
-      <c r="B6" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="7">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
-      <c r="B7" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
-      <c r="B8" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="7"/>
-    </row>
-    <row r="10" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="27"/>
-      <c r="B10" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="7"/>
-    </row>
-    <row r="11" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="27"/>
-      <c r="B11" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="7"/>
-    </row>
-    <row r="12" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="29"/>
-      <c r="B13" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="31"/>
-      <c r="B15" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A4:A8"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A14:A15"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter>
-    <oddHeader>&amp;R&amp;"Calibri"&amp;8&amp;K808080 INTERNAL &amp; PARTNERS&amp;1#_x000D_</oddHeader>
-    <oddFooter>&amp;R_x000D_&amp;1#&amp;"Calibri"&amp;2&amp;KFFFFFF 5acXjzUk</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -8047,7 +7914,291 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2A86181-EF33-48DD-ABA9-ABF62C32FC08}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="29">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="29">
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:C1" xr:uid="{E2A86181-EF33-48DD-ABA9-ABF62C32FC08}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C322632-4B48-4009-913B-945F1E0D549C}">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="30" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="29" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="29" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="29" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="29" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="31"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" style="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="33"/>
+      <c r="B3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="7">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="33"/>
+      <c r="B5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="33"/>
+      <c r="B6" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="33"/>
+      <c r="B7" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="33"/>
+      <c r="B8" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="7"/>
+    </row>
+    <row r="10" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="33"/>
+      <c r="B10" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="7"/>
+    </row>
+    <row r="11" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="33"/>
+      <c r="B11" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="7"/>
+    </row>
+    <row r="12" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="35"/>
+      <c r="B13" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="37"/>
+      <c r="B15" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddHeader>&amp;R&amp;"Calibri"&amp;8&amp;K808080 INTERNAL &amp; PARTNERS&amp;1#_x000D_</oddHeader>
+    <oddFooter>&amp;R_x000D_&amp;1#&amp;"Calibri"&amp;2&amp;KFFFFFF 5acXjzUk</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>

</xml_diff>

<commit_message>
New feature : can duplicate machines
</commit_message>
<xml_diff>
--- a/LineData.xlsx
+++ b/LineData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danislud\Documents\PRODynamics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F4DC0A4F-DB1B-486D-9D85-57D5B0E25082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{22B5F35C-0123-4E02-ACC2-337C6BBB4BEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Line Data" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="78">
   <si>
     <t>Available Strategies</t>
   </si>
@@ -260,6 +260,9 @@
   <si>
     <t>Quantity</t>
   </si>
+  <si>
+    <t>Duplicate</t>
+  </si>
 </sst>
 </file>
 
@@ -326,7 +329,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -495,11 +498,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -597,6 +613,15 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -985,10 +1010,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:N481"/>
+  <dimension ref="A1:O481"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1006,10 +1031,10 @@
     <col min="11" max="11" width="18.42578125" style="23" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18.42578125" style="23" customWidth="1"/>
     <col min="13" max="13" width="15.42578125" style="22" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>3</v>
       </c>
@@ -1052,8 +1077,11 @@
       <c r="N1" s="27" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O1" s="38" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>8</v>
       </c>
@@ -1094,8 +1122,11 @@
       <c r="N2" s="28" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O2" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>9</v>
       </c>
@@ -1133,11 +1164,14 @@
         <v>0</v>
       </c>
       <c r="M3" s="25"/>
-      <c r="N3" s="26" t="b">
+      <c r="N3" s="37" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O3" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>10</v>
       </c>
@@ -1175,11 +1209,14 @@
         <v>0</v>
       </c>
       <c r="M4" s="25"/>
-      <c r="N4" s="26" t="b">
+      <c r="N4" s="37" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O4" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>11</v>
       </c>
@@ -1217,11 +1254,14 @@
         <v>0</v>
       </c>
       <c r="M5" s="25"/>
-      <c r="N5" s="26" t="b">
+      <c r="N5" s="37" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O5" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>12</v>
       </c>
@@ -1259,11 +1299,14 @@
         <v>0</v>
       </c>
       <c r="M6" s="25"/>
-      <c r="N6" s="26" t="b">
+      <c r="N6" s="37" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O6" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>13</v>
       </c>
@@ -1301,11 +1344,14 @@
         <v>0</v>
       </c>
       <c r="M7" s="25"/>
-      <c r="N7" s="26" t="b">
+      <c r="N7" s="37" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O7" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>14</v>
       </c>
@@ -1343,11 +1389,14 @@
         <v>0</v>
       </c>
       <c r="M8" s="25"/>
-      <c r="N8" s="26" t="b">
+      <c r="N8" s="37" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O8" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>15</v>
       </c>
@@ -1385,11 +1434,14 @@
         <v>0</v>
       </c>
       <c r="M9" s="25"/>
-      <c r="N9" s="26" t="b">
+      <c r="N9" s="37" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O9" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>16</v>
       </c>
@@ -1427,11 +1479,14 @@
         <v>0</v>
       </c>
       <c r="M10" s="25"/>
-      <c r="N10" s="26" t="b">
+      <c r="N10" s="37" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O10" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>17</v>
       </c>
@@ -1469,11 +1524,14 @@
         <v>0</v>
       </c>
       <c r="M11" s="25"/>
-      <c r="N11" s="26" t="b">
+      <c r="N11" s="37" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O11" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>18</v>
       </c>
@@ -1511,11 +1569,14 @@
         <v>0</v>
       </c>
       <c r="M12" s="25"/>
-      <c r="N12" s="26" t="b">
+      <c r="N12" s="37" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O12" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>19</v>
       </c>
@@ -1553,11 +1614,14 @@
         <v>0</v>
       </c>
       <c r="M13" s="25"/>
-      <c r="N13" s="26" t="b">
+      <c r="N13" s="37" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O13" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>20</v>
       </c>
@@ -1595,11 +1659,14 @@
         <v>0</v>
       </c>
       <c r="M14" s="25"/>
-      <c r="N14" s="26" t="b">
+      <c r="N14" s="37" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O14" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1612,7 +1679,7 @@
       <c r="J15" s="4"/>
       <c r="M15" s="21"/>
     </row>
-    <row r="16" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -7904,7 +7971,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2A86181-EF33-48DD-ABA9-ABF62C32FC08}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>

</xml_diff>